<commit_message>
unit 73 and unit 74
</commit_message>
<xml_diff>
--- a/homework/74.xlsx
+++ b/homework/74.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFBADBE-6178-42A4-9364-FA1FB6287D20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5352288E-D6AC-4F83-AB66-1CC3A0FF3681}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4890" yWindow="2985" windowWidth="23910" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13470" yWindow="2820" windowWidth="15330" windowHeight="10725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>73.2</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -42,6 +42,125 @@
   </si>
   <si>
     <t>the Kenyas(Kenya)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The United States</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>the Andes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bangkok</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The Alps</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>the Bahamas</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>the</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Jamaica</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kenya(the red sea)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>the Regal Cinema</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>the Museum of Art</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>the Mississippi or the Nile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>the Park Hotel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The west of Ireland</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>the Panama Canal , the atlantic Ocean , the Pacific Ocean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The Rocky Mountains , </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>North America</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>the london(the national Gallery)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ok(the netherlands)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ok(the south of france)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ok(the philippines)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -49,7 +168,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,6 +192,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <name val="宋体"/>
       <family val="3"/>
@@ -106,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -120,6 +247,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -461,7 +589,7 @@
   <dimension ref="A3:D86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -538,49 +666,63 @@
       <c r="B10" s="6">
         <v>9</v>
       </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="6" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="5"/>
       <c r="B11" s="6">
         <v>10</v>
       </c>
-      <c r="C11" s="6"/>
+      <c r="C11" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" s="5"/>
       <c r="B12" s="6">
         <v>11</v>
       </c>
-      <c r="C12" s="6"/>
+      <c r="C12" s="6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="5"/>
       <c r="B13" s="6">
         <v>12</v>
       </c>
-      <c r="C13" s="6"/>
+      <c r="C13" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="5"/>
       <c r="B14" s="6">
         <v>13</v>
       </c>
-      <c r="C14" s="7"/>
+      <c r="C14" s="8" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="5"/>
       <c r="B15" s="6">
         <v>14</v>
       </c>
-      <c r="C15" s="6"/>
+      <c r="C15" s="9" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" s="5"/>
       <c r="B16" s="6">
         <v>15</v>
       </c>
-      <c r="C16" s="6"/>
+      <c r="C16" s="6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="5"/>
@@ -599,91 +741,117 @@
       <c r="B19" s="6">
         <v>3</v>
       </c>
-      <c r="C19" s="6"/>
+      <c r="C19" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="5"/>
       <c r="B20" s="6">
         <v>4</v>
       </c>
-      <c r="C20" s="6"/>
+      <c r="C20" s="8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="5"/>
       <c r="B21" s="6">
         <v>5</v>
       </c>
-      <c r="C21" s="6"/>
+      <c r="C21" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="5"/>
       <c r="B22" s="6">
         <v>6</v>
       </c>
-      <c r="C22" s="6"/>
+      <c r="C22" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="5"/>
       <c r="B23" s="6">
         <v>7</v>
       </c>
-      <c r="C23" s="6"/>
+      <c r="C23" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="5"/>
       <c r="B24" s="6">
         <v>8</v>
       </c>
-      <c r="C24" s="6"/>
+      <c r="C24" s="6" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="5"/>
       <c r="B25" s="6">
         <v>9</v>
       </c>
-      <c r="C25" s="6"/>
+      <c r="C25" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="5"/>
       <c r="B26" s="6">
         <v>10</v>
       </c>
-      <c r="C26" s="6"/>
+      <c r="C26" s="8" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="5"/>
       <c r="B27" s="6">
         <v>11</v>
       </c>
-      <c r="C27" s="6"/>
+      <c r="C27" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="5"/>
       <c r="B28" s="6">
         <v>12</v>
       </c>
-      <c r="C28" s="6"/>
+      <c r="C28" s="8" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="5"/>
       <c r="B29" s="6">
         <v>13</v>
       </c>
-      <c r="C29" s="6"/>
+      <c r="C29" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" s="5"/>
       <c r="B30" s="6">
         <v>14</v>
       </c>
-      <c r="C30" s="6"/>
+      <c r="C30" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="5"/>
       <c r="B31" s="6">
         <v>15</v>
       </c>
-      <c r="C31" s="6"/>
+      <c r="C31" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="D31" s="3"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
@@ -691,35 +859,45 @@
       <c r="B32" s="6">
         <v>16</v>
       </c>
-      <c r="C32" s="6"/>
+      <c r="C32" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" s="5"/>
       <c r="B33" s="6">
         <v>17</v>
       </c>
-      <c r="C33" s="6"/>
+      <c r="C33" s="6" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" s="5"/>
       <c r="B34" s="6">
         <v>18</v>
       </c>
-      <c r="C34" s="6"/>
+      <c r="C34" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" s="5"/>
       <c r="B35" s="6">
         <v>19</v>
       </c>
-      <c r="C35" s="6"/>
+      <c r="C35" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" s="5"/>
       <c r="B36" s="6">
         <v>20</v>
       </c>
-      <c r="C36" s="6"/>
+      <c r="C36" s="6" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" s="5"/>

</xml_diff>